<commit_message>
Add Tinas maybe temp files
</commit_message>
<xml_diff>
--- a/Lab 2 Rubric.xlsx
+++ b/Lab 2 Rubric.xlsx
@@ -1,39 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bblanchard006/Desktop/SMU/Data Mining 7331 Class Materials v1/Class 7/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tina/Documents/School/ML1/SMUMSDS-ML1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{03DA96D3-7215-464D-8BFA-98B3686FB84E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D48F3B-D4FD-8146-B1D8-F087E664551E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" xr2:uid="{AA98FEFF-5C75-5143-BD21-4AF18B1BA09F}"/>
+    <workbookView xWindow="6380" yWindow="2340" windowWidth="21900" windowHeight="14420" xr2:uid="{AA98FEFF-5C75-5143-BD21-4AF18B1BA09F}"/>
   </bookViews>
   <sheets>
     <sheet name="Group #" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Rubric</t>
   </si>
@@ -117,6 +109,12 @@
   </si>
   <si>
     <t>Choose the method you will use for dividing your data into training and testing splits (i.e., are you using Stratified 10-fold cross validation? Why?). Explain why your chosen method is appropriate or use more than one method as appropriate. For example, if you are using time series data then you should be using continuous training and testing sets across time.</t>
+  </si>
+  <si>
+    <t>Task 1</t>
+  </si>
+  <si>
+    <t>Task 2</t>
   </si>
 </sst>
 </file>
@@ -565,208 +563,214 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47E02241-AB49-454D-AC4B-EC1C6B4EA63C}">
-  <dimension ref="B1:F13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="3" topLeftCell="F11" activePane="bottomRight" state="frozen"/>
       <selection activeCell="F2" sqref="F2:F3"/>
       <selection pane="topRight" activeCell="F2" sqref="F2:F3"/>
       <selection pane="bottomLeft" activeCell="F2" sqref="F2:F3"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="6"/>
-    <col min="2" max="2" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="58.6640625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="58.6640625" style="6" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="6"/>
+    <col min="1" max="2" width="10.83203125" style="6"/>
+    <col min="3" max="3" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="58.6640625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="58.6640625" style="6" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C1" s="2" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="D2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="4">
+      <c r="E2" s="4">
         <v>20</v>
       </c>
-      <c r="E2" s="5">
-        <f>(E3/100)*$D$2</f>
+      <c r="F2" s="5">
+        <f>(F3/100)*$E$2</f>
         <v>0</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="G2" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B3" s="3" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="4">
-        <f>SUM(D4:D13)</f>
+      <c r="D3" s="12"/>
+      <c r="E3" s="4">
+        <f>SUM(E4:E13)</f>
         <v>100</v>
       </c>
-      <c r="E3" s="5">
-        <f>SUM(E4:E13)</f>
+      <c r="F3" s="5">
+        <f>SUM(F4:F13)</f>
         <v>0</v>
       </c>
-      <c r="F3" s="12"/>
-    </row>
-    <row r="4" spans="2:6" ht="68" x14ac:dyDescent="0.2">
-      <c r="B4" s="3" t="s">
+      <c r="G3" s="12"/>
+    </row>
+    <row r="4" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="D4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="8">
+      <c r="E4" s="8">
         <v>10</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="7"/>
-    </row>
-    <row r="5" spans="2:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="B5" s="3" t="s">
+      <c r="F4" s="9"/>
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="D5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="8">
+      <c r="E5" s="8">
         <v>5</v>
       </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="2:6" ht="85" x14ac:dyDescent="0.2">
-      <c r="B6" s="3" t="s">
+      <c r="F5" s="9"/>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="8">
+      <c r="E6" s="8">
         <v>10</v>
       </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="7"/>
-    </row>
-    <row r="7" spans="2:6" ht="102" x14ac:dyDescent="0.2">
-      <c r="B7" s="3" t="s">
+      <c r="F6" s="9"/>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="C7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="D7" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="8">
+      <c r="E7" s="8">
         <v>10</v>
       </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="7"/>
-    </row>
-    <row r="8" spans="2:6" ht="119" x14ac:dyDescent="0.2">
-      <c r="B8" s="3" t="s">
+      <c r="F7" s="9"/>
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+      <c r="C8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="D8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="8">
+      <c r="E8" s="8">
         <v>20</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="2:6" ht="68" x14ac:dyDescent="0.2">
-      <c r="B9" s="3" t="s">
+      <c r="F8" s="9"/>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="C9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="D9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="8">
+      <c r="E9" s="8">
         <v>10</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="7"/>
-    </row>
-    <row r="10" spans="2:6" ht="102" x14ac:dyDescent="0.2">
-      <c r="B10" s="3" t="s">
+      <c r="F9" s="9"/>
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="C10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="D10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="8">
+      <c r="E10" s="8">
         <v>10</v>
       </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="7"/>
-    </row>
-    <row r="11" spans="2:6" ht="85" x14ac:dyDescent="0.2">
-      <c r="B11" s="3" t="s">
+      <c r="F10" s="9"/>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="C11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="D11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="8">
+      <c r="E11" s="8">
         <v>10</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="7"/>
-    </row>
-    <row r="12" spans="2:6" ht="102" x14ac:dyDescent="0.2">
-      <c r="B12" s="3" t="s">
+      <c r="F11" s="9"/>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="C12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="D12" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="8">
+      <c r="E12" s="8">
         <v>5</v>
       </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="7"/>
-    </row>
-    <row r="13" spans="2:6" ht="85" x14ac:dyDescent="0.2">
-      <c r="B13" s="3" t="s">
+      <c r="F12" s="9"/>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="C13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="D13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="8">
+      <c r="E13" s="8">
         <v>10</v>
       </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="7"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="G2:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>